<commit_message>
Student Sort, Frequency, Average
Finished Student Sort, Frequency, Average.
Only 1 dictionary exists for projects.
However, 2 dictionaries exist for students. 1 for project preferences and 1 for specifications.

Student file converted into excel file. Code expects excel file as input file. Code will not work with csvs for students. New excel files created and 1.02 companies excel changed to help make algorithm.

Changed NAs in GPA in students to 2s.
</commit_message>
<xml_diff>
--- a/Samples/EE 364D Project Assignment Survey (Fall 2022)-v116-to team-out.xlsx
+++ b/Samples/EE 364D Project Assignment Survey (Fall 2022)-v116-to team-out.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a598a8a5c4798f14/Desktop/Senior_Design/UT-Student-Assignment/Samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\UT-Student-Assignment\Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{04B24614-7AF0-4FD5-8EC5-E347E71B9024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF9C58C7-4581-437F-A8E3-358D2AB10853}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F12F2C-88D2-4AD7-AE58-C987E9C1C28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-180" yWindow="0" windowWidth="10515" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AnonData" sheetId="3" r:id="rId1"/>
@@ -2950,9 +2950,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2990,7 +2990,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3096,7 +3096,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3238,7 +3238,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3248,87 +3248,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F28E219-EBEA-48C9-A5B8-2119E887BCFF}">
   <dimension ref="A1:BU195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="12660" ySplit="4050" topLeftCell="BU1"/>
-      <selection activeCell="F1" sqref="F1"/>
-      <selection pane="topRight" activeCell="BF37" sqref="BF37"/>
-      <selection pane="bottomLeft" activeCell="A103" sqref="A103"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="BS1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BT1" sqref="BT1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="5.58203125" customWidth="1"/>
-    <col min="5" max="5" width="7.4140625" customWidth="1"/>
-    <col min="6" max="6" width="91.4140625" customWidth="1"/>
-    <col min="7" max="7" width="50.08203125" customWidth="1"/>
-    <col min="8" max="8" width="30.9140625" customWidth="1"/>
+    <col min="4" max="4" width="5.625" customWidth="1"/>
+    <col min="5" max="5" width="7.375" customWidth="1"/>
+    <col min="6" max="6" width="91.375" customWidth="1"/>
+    <col min="7" max="7" width="50.125" customWidth="1"/>
+    <col min="8" max="8" width="30.875" customWidth="1"/>
     <col min="9" max="9" width="34.5" customWidth="1"/>
     <col min="10" max="10" width="38.75" customWidth="1"/>
-    <col min="11" max="11" width="34.9140625" customWidth="1"/>
-    <col min="12" max="12" width="42.33203125" customWidth="1"/>
-    <col min="13" max="13" width="38.6640625" customWidth="1"/>
+    <col min="11" max="11" width="34.875" customWidth="1"/>
+    <col min="12" max="12" width="42.375" customWidth="1"/>
+    <col min="13" max="13" width="38.625" customWidth="1"/>
     <col min="14" max="14" width="30" customWidth="1"/>
-    <col min="15" max="15" width="24.1640625" customWidth="1"/>
-    <col min="16" max="16" width="23.9140625" customWidth="1"/>
+    <col min="15" max="15" width="24.125" customWidth="1"/>
+    <col min="16" max="16" width="23.875" customWidth="1"/>
     <col min="17" max="17" width="25" customWidth="1"/>
-    <col min="18" max="19" width="24.6640625" customWidth="1"/>
-    <col min="20" max="20" width="25.83203125" customWidth="1"/>
-    <col min="21" max="21" width="25.4140625" customWidth="1"/>
-    <col min="22" max="22" width="25.6640625" customWidth="1"/>
+    <col min="18" max="19" width="24.625" customWidth="1"/>
+    <col min="20" max="20" width="25.875" customWidth="1"/>
+    <col min="21" max="21" width="25.375" customWidth="1"/>
+    <col min="22" max="22" width="25.625" customWidth="1"/>
     <col min="23" max="23" width="26.5" customWidth="1"/>
     <col min="24" max="24" width="40.5" customWidth="1"/>
-    <col min="25" max="25" width="29.4140625" customWidth="1"/>
-    <col min="26" max="26" width="25.4140625" customWidth="1"/>
-    <col min="27" max="27" width="25.9140625" customWidth="1"/>
+    <col min="25" max="25" width="29.375" customWidth="1"/>
+    <col min="26" max="26" width="25.375" customWidth="1"/>
+    <col min="27" max="27" width="25.875" customWidth="1"/>
     <col min="28" max="28" width="24.5" customWidth="1"/>
-    <col min="29" max="29" width="25.83203125" customWidth="1"/>
-    <col min="30" max="30" width="25.6640625" customWidth="1"/>
-    <col min="31" max="31" width="23.1640625" customWidth="1"/>
-    <col min="32" max="32" width="25.83203125" customWidth="1"/>
-    <col min="33" max="33" width="25.1640625" customWidth="1"/>
-    <col min="34" max="34" width="25.58203125" customWidth="1"/>
-    <col min="35" max="35" width="25.33203125" customWidth="1"/>
-    <col min="36" max="36" width="24.33203125" customWidth="1"/>
-    <col min="37" max="37" width="25.4140625" customWidth="1"/>
-    <col min="38" max="38" width="23.58203125" customWidth="1"/>
-    <col min="39" max="39" width="23.9140625" customWidth="1"/>
-    <col min="40" max="40" width="21.9140625" customWidth="1"/>
+    <col min="29" max="29" width="25.875" customWidth="1"/>
+    <col min="30" max="30" width="25.625" customWidth="1"/>
+    <col min="31" max="31" width="23.125" customWidth="1"/>
+    <col min="32" max="32" width="25.875" customWidth="1"/>
+    <col min="33" max="33" width="25.125" customWidth="1"/>
+    <col min="34" max="34" width="25.625" customWidth="1"/>
+    <col min="35" max="35" width="25.375" customWidth="1"/>
+    <col min="36" max="36" width="24.375" customWidth="1"/>
+    <col min="37" max="37" width="25.375" customWidth="1"/>
+    <col min="38" max="38" width="23.625" customWidth="1"/>
+    <col min="39" max="39" width="23.875" customWidth="1"/>
+    <col min="40" max="40" width="21.875" customWidth="1"/>
     <col min="41" max="41" width="25.75" customWidth="1"/>
-    <col min="42" max="42" width="26.4140625" customWidth="1"/>
-    <col min="43" max="43" width="21.9140625" customWidth="1"/>
-    <col min="44" max="44" width="22.33203125" customWidth="1"/>
+    <col min="42" max="42" width="26.375" customWidth="1"/>
+    <col min="43" max="43" width="21.875" customWidth="1"/>
+    <col min="44" max="44" width="22.375" customWidth="1"/>
     <col min="45" max="45" width="12.5" customWidth="1"/>
-    <col min="46" max="46" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="23.1640625" customWidth="1"/>
-    <col min="48" max="48" width="24.08203125" customWidth="1"/>
+    <col min="46" max="46" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="23.125" customWidth="1"/>
+    <col min="48" max="48" width="24.125" customWidth="1"/>
     <col min="49" max="51" width="22.75" customWidth="1"/>
-    <col min="52" max="52" width="23.83203125" customWidth="1"/>
-    <col min="53" max="53" width="25.4140625" customWidth="1"/>
-    <col min="54" max="54" width="25.6640625" customWidth="1"/>
-    <col min="55" max="55" width="24.4140625" customWidth="1"/>
-    <col min="56" max="56" width="24.83203125" customWidth="1"/>
-    <col min="57" max="58" width="24.1640625" customWidth="1"/>
-    <col min="59" max="59" width="25.58203125" customWidth="1"/>
-    <col min="60" max="60" width="25.1640625" customWidth="1"/>
-    <col min="61" max="61" width="24.58203125" customWidth="1"/>
-    <col min="62" max="62" width="24.9140625" customWidth="1"/>
-    <col min="63" max="63" width="25.33203125" customWidth="1"/>
+    <col min="52" max="52" width="23.875" customWidth="1"/>
+    <col min="53" max="53" width="25.375" customWidth="1"/>
+    <col min="54" max="54" width="25.625" customWidth="1"/>
+    <col min="55" max="55" width="24.375" customWidth="1"/>
+    <col min="56" max="56" width="24.875" customWidth="1"/>
+    <col min="57" max="58" width="24.125" customWidth="1"/>
+    <col min="59" max="59" width="25.625" customWidth="1"/>
+    <col min="60" max="60" width="25.125" customWidth="1"/>
+    <col min="61" max="61" width="24.625" customWidth="1"/>
+    <col min="62" max="62" width="24.875" customWidth="1"/>
+    <col min="63" max="63" width="25.375" customWidth="1"/>
     <col min="64" max="64" width="23.75" customWidth="1"/>
-    <col min="65" max="65" width="24.9140625" customWidth="1"/>
-    <col min="66" max="66" width="2.83203125" customWidth="1"/>
-    <col min="67" max="67" width="2.58203125" customWidth="1"/>
-    <col min="68" max="68" width="2.25" customWidth="1"/>
-    <col min="69" max="69" width="2.33203125" customWidth="1"/>
-    <col min="70" max="70" width="2.08203125" customWidth="1"/>
-    <col min="71" max="71" width="2.4140625" customWidth="1"/>
-    <col min="72" max="72" width="1.83203125" customWidth="1"/>
-    <col min="73" max="73" width="87.1640625" customWidth="1"/>
+    <col min="65" max="65" width="24.875" customWidth="1"/>
+    <col min="66" max="66" width="134" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="147" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="71.375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="52.125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="100.75" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="91.5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="87.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" s="1" customFormat="1" ht="255.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:73" s="1" customFormat="1" ht="255.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3546,7 +3542,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>326</v>
       </c>
@@ -3755,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>327</v>
       </c>
@@ -3967,7 +3963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -4179,7 +4175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>329</v>
       </c>
@@ -4395,7 +4391,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>330</v>
       </c>
@@ -4611,7 +4607,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>331</v>
       </c>
@@ -4826,7 +4822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>332</v>
       </c>
@@ -5045,7 +5041,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>333</v>
       </c>
@@ -5261,7 +5257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>334</v>
       </c>
@@ -5479,7 +5475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>335</v>
       </c>
@@ -5697,7 +5693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>336</v>
       </c>
@@ -5909,7 +5905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>337</v>
       </c>
@@ -6124,7 +6120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>338</v>
       </c>
@@ -6337,7 +6333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>339</v>
       </c>
@@ -6553,7 +6549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>340</v>
       </c>
@@ -6765,7 +6761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>341</v>
       </c>
@@ -6978,7 +6974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>342</v>
       </c>
@@ -7194,7 +7190,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>343</v>
       </c>
@@ -7406,7 +7402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>344</v>
       </c>
@@ -7625,7 +7621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>345</v>
       </c>
@@ -7841,7 +7837,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>346</v>
       </c>
@@ -8059,7 +8055,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>347</v>
       </c>
@@ -8275,7 +8271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>348</v>
       </c>
@@ -8490,7 +8486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>349</v>
       </c>
@@ -8708,7 +8704,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>350</v>
       </c>
@@ -8923,7 +8919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>351</v>
       </c>
@@ -9138,7 +9134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>352</v>
       </c>
@@ -9354,7 +9350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>353</v>
       </c>
@@ -9569,7 +9565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>354</v>
       </c>
@@ -9785,7 +9781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>355</v>
       </c>
@@ -10000,7 +9996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>356</v>
       </c>
@@ -10215,7 +10211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>357</v>
       </c>
@@ -10433,7 +10429,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>358</v>
       </c>
@@ -10651,7 +10647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>359</v>
       </c>
@@ -10867,7 +10863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>360</v>
       </c>
@@ -11083,7 +11079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>361</v>
       </c>
@@ -11295,7 +11291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>362</v>
       </c>
@@ -11507,7 +11503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>363</v>
       </c>
@@ -11723,7 +11719,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>364</v>
       </c>
@@ -11942,7 +11938,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>365</v>
       </c>
@@ -12160,7 +12156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>366</v>
       </c>
@@ -12372,7 +12368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>367</v>
       </c>
@@ -12585,7 +12581,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>368</v>
       </c>
@@ -12801,7 +12797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>369</v>
       </c>
@@ -13014,7 +13010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>370</v>
       </c>
@@ -13226,7 +13222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>371</v>
       </c>
@@ -13445,7 +13441,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>372</v>
       </c>
@@ -13660,7 +13656,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>373</v>
       </c>
@@ -13872,7 +13868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>374</v>
       </c>
@@ -14090,7 +14086,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>375</v>
       </c>
@@ -14305,7 +14301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>376</v>
       </c>
@@ -14521,7 +14517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>377</v>
       </c>
@@ -14740,7 +14736,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>378</v>
       </c>
@@ -14959,7 +14955,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>379</v>
       </c>
@@ -15175,7 +15171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>380</v>
       </c>
@@ -15394,7 +15390,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>381</v>
       </c>
@@ -15609,7 +15605,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>382</v>
       </c>
@@ -15821,7 +15817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>383</v>
       </c>
@@ -16036,7 +16032,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>384</v>
       </c>
@@ -16252,7 +16248,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>385</v>
       </c>
@@ -16464,7 +16460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>386</v>
       </c>
@@ -16680,7 +16676,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>387</v>
       </c>
@@ -16899,7 +16895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>388</v>
       </c>
@@ -17113,7 +17109,7 @@
       </c>
       <c r="BU64" s="3"/>
     </row>
-    <row r="65" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>389</v>
       </c>
@@ -17328,7 +17324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>390</v>
       </c>
@@ -17546,7 +17542,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>391</v>
       </c>
@@ -17762,7 +17758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>392</v>
       </c>
@@ -17977,7 +17973,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:73" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:73" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>393</v>
       </c>
@@ -18192,7 +18188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>394</v>
       </c>
@@ -18412,7 +18408,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>395</v>
       </c>
@@ -18627,7 +18623,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>396</v>
       </c>
@@ -18843,7 +18839,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>397</v>
       </c>
@@ -19056,7 +19052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>398</v>
       </c>
@@ -19271,7 +19267,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>399</v>
       </c>
@@ -19487,7 +19483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>400</v>
       </c>
@@ -19705,7 +19701,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="77" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>401</v>
       </c>
@@ -19918,7 +19914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>402</v>
       </c>
@@ -20131,7 +20127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>403</v>
       </c>
@@ -20344,7 +20340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>404</v>
       </c>
@@ -20557,7 +20553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>405</v>
       </c>
@@ -20770,7 +20766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>406</v>
       </c>
@@ -20989,7 +20985,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>407</v>
       </c>
@@ -21205,7 +21201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>408</v>
       </c>
@@ -21418,7 +21414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:73" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:73" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>409</v>
       </c>
@@ -21634,7 +21630,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>410</v>
       </c>
@@ -21849,7 +21845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>411</v>
       </c>
@@ -22055,7 +22051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>412</v>
       </c>
@@ -22271,7 +22267,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>413</v>
       </c>
@@ -22487,7 +22483,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="90" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>414</v>
       </c>
@@ -22700,7 +22696,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="91" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>415</v>
       </c>
@@ -22916,7 +22912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>416</v>
       </c>
@@ -23128,7 +23124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:73" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:73" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>417</v>
       </c>
@@ -23341,7 +23337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>418</v>
       </c>
@@ -23556,7 +23552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>419</v>
       </c>
@@ -23769,7 +23765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:73" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:73" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>420</v>
       </c>
@@ -23982,7 +23978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>421</v>
       </c>
@@ -24195,7 +24191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>422</v>
       </c>
@@ -24399,7 +24395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>423</v>
       </c>
@@ -24611,7 +24607,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>424</v>
       </c>
@@ -24830,7 +24826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:73" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:73" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BN101" s="3"/>
       <c r="BO101" s="3"/>
       <c r="BP101" s="3"/>
@@ -24839,7 +24835,7 @@
       <c r="BS101" s="3"/>
       <c r="BT101" s="3"/>
     </row>
-    <row r="102" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN102" s="3"/>
       <c r="BO102" s="3"/>
       <c r="BP102" s="3"/>
@@ -24848,7 +24844,7 @@
       <c r="BS102" s="3"/>
       <c r="BT102" s="3"/>
     </row>
-    <row r="103" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN103" s="3"/>
       <c r="BO103" s="3"/>
       <c r="BP103" s="3"/>
@@ -24857,7 +24853,7 @@
       <c r="BS103" s="3"/>
       <c r="BT103" s="3"/>
     </row>
-    <row r="104" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN104" s="3"/>
       <c r="BO104" s="3"/>
       <c r="BP104" s="3"/>
@@ -24866,7 +24862,7 @@
       <c r="BS104" s="3"/>
       <c r="BT104" s="3"/>
     </row>
-    <row r="105" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN105" s="3"/>
       <c r="BO105" s="3"/>
       <c r="BP105" s="3"/>
@@ -24875,7 +24871,7 @@
       <c r="BS105" s="3"/>
       <c r="BT105" s="3"/>
     </row>
-    <row r="106" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN106" s="3"/>
       <c r="BO106" s="3"/>
       <c r="BP106" s="3"/>
@@ -24884,7 +24880,7 @@
       <c r="BS106" s="3"/>
       <c r="BT106" s="3"/>
     </row>
-    <row r="107" spans="1:73" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:73" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10"/>
       <c r="B107" s="10"/>
       <c r="C107" s="10"/>
@@ -24899,7 +24895,7 @@
       <c r="BS107" s="3"/>
       <c r="BT107" s="3"/>
     </row>
-    <row r="108" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A108" s="10"/>
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
@@ -24914,7 +24910,7 @@
       <c r="BS108" s="3"/>
       <c r="BT108" s="3"/>
     </row>
-    <row r="109" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A109" s="10"/>
       <c r="B109" s="10"/>
       <c r="C109" s="10"/>
@@ -24929,7 +24925,7 @@
       <c r="BS109" s="3"/>
       <c r="BT109" s="3"/>
     </row>
-    <row r="110" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A110" s="10"/>
       <c r="B110" s="10"/>
       <c r="C110" s="10"/>
@@ -24944,7 +24940,7 @@
       <c r="BS110" s="3"/>
       <c r="BT110" s="3"/>
     </row>
-    <row r="111" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A111" s="10"/>
       <c r="B111" s="10"/>
       <c r="C111" s="10"/>
@@ -24959,7 +24955,7 @@
       <c r="BS111" s="3"/>
       <c r="BT111" s="3"/>
     </row>
-    <row r="112" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
@@ -24974,7 +24970,7 @@
       <c r="BS112" s="3"/>
       <c r="BT112" s="3"/>
     </row>
-    <row r="113" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
@@ -24989,7 +24985,7 @@
       <c r="BS113" s="3"/>
       <c r="BT113" s="3"/>
     </row>
-    <row r="114" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN114" s="3"/>
       <c r="BO114" s="3"/>
       <c r="BP114" s="3"/>
@@ -24998,7 +24994,7 @@
       <c r="BS114" s="3"/>
       <c r="BT114" s="3"/>
     </row>
-    <row r="115" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN115" s="3"/>
       <c r="BO115" s="3"/>
       <c r="BP115" s="3"/>
@@ -25007,7 +25003,7 @@
       <c r="BS115" s="3"/>
       <c r="BT115" s="3"/>
     </row>
-    <row r="116" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN116" s="3"/>
       <c r="BO116" s="3"/>
       <c r="BP116" s="3"/>
@@ -25016,7 +25012,7 @@
       <c r="BS116" s="3"/>
       <c r="BT116" s="3"/>
     </row>
-    <row r="117" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN117" s="3"/>
       <c r="BO117" s="3"/>
       <c r="BP117" s="3"/>
@@ -25025,7 +25021,7 @@
       <c r="BS117" s="3"/>
       <c r="BT117" s="3"/>
     </row>
-    <row r="118" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BN118" s="3"/>
       <c r="BO118" s="3"/>
       <c r="BP118" s="3"/>
@@ -25034,7 +25030,7 @@
       <c r="BS118" s="3"/>
       <c r="BT118" s="3"/>
     </row>
-    <row r="119" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN119" s="3"/>
       <c r="BO119" s="3"/>
       <c r="BP119" s="3"/>
@@ -25043,7 +25039,7 @@
       <c r="BS119" s="3"/>
       <c r="BT119" s="3"/>
     </row>
-    <row r="120" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A120" s="10"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
@@ -25058,7 +25054,7 @@
       <c r="BS120" s="3"/>
       <c r="BT120" s="3"/>
     </row>
-    <row r="121" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
       <c r="B121" s="10"/>
       <c r="C121" s="10"/>
@@ -25073,7 +25069,7 @@
       <c r="BS121" s="3"/>
       <c r="BT121" s="3"/>
     </row>
-    <row r="122" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
@@ -25088,7 +25084,7 @@
       <c r="BS122" s="3"/>
       <c r="BT122" s="3"/>
     </row>
-    <row r="123" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A123" s="10"/>
       <c r="B123" s="10"/>
       <c r="C123" s="10"/>
@@ -25103,7 +25099,7 @@
       <c r="BS123" s="3"/>
       <c r="BT123" s="3"/>
     </row>
-    <row r="124" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A124" s="10"/>
       <c r="B124" s="10"/>
       <c r="C124" s="10"/>
@@ -25118,7 +25114,7 @@
       <c r="BS124" s="3"/>
       <c r="BT124" s="3"/>
     </row>
-    <row r="125" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN125" s="3"/>
       <c r="BO125" s="3"/>
       <c r="BP125" s="3"/>
@@ -25127,7 +25123,7 @@
       <c r="BS125" s="3"/>
       <c r="BT125" s="3"/>
     </row>
-    <row r="126" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN126" s="3"/>
       <c r="BO126" s="3"/>
       <c r="BP126" s="3"/>
@@ -25136,7 +25132,7 @@
       <c r="BS126" s="3"/>
       <c r="BT126" s="3"/>
     </row>
-    <row r="127" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN127" s="3"/>
       <c r="BO127" s="3"/>
       <c r="BP127" s="3"/>
@@ -25145,7 +25141,7 @@
       <c r="BS127" s="3"/>
       <c r="BT127" s="3"/>
     </row>
-    <row r="128" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN128" s="3"/>
       <c r="BO128" s="3"/>
       <c r="BP128" s="3"/>
@@ -25154,7 +25150,7 @@
       <c r="BS128" s="3"/>
       <c r="BT128" s="3"/>
     </row>
-    <row r="129" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN129" s="3"/>
       <c r="BO129" s="3"/>
       <c r="BP129" s="3"/>
@@ -25163,7 +25159,7 @@
       <c r="BS129" s="3"/>
       <c r="BT129" s="3"/>
     </row>
-    <row r="130" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
       <c r="B130" s="10"/>
       <c r="C130" s="10"/>
@@ -25178,7 +25174,7 @@
       <c r="BS130" s="3"/>
       <c r="BT130" s="3"/>
     </row>
-    <row r="131" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A131" s="10"/>
       <c r="B131" s="10"/>
       <c r="C131" s="10"/>
@@ -25193,7 +25189,7 @@
       <c r="BS131" s="3"/>
       <c r="BT131" s="3"/>
     </row>
-    <row r="132" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A132" s="10"/>
       <c r="B132" s="10"/>
       <c r="C132" s="10"/>
@@ -25208,7 +25204,7 @@
       <c r="BS132" s="3"/>
       <c r="BT132" s="3"/>
     </row>
-    <row r="133" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A133" s="10"/>
       <c r="B133" s="10"/>
       <c r="C133" s="10"/>
@@ -25223,7 +25219,7 @@
       <c r="BS133" s="3"/>
       <c r="BT133" s="3"/>
     </row>
-    <row r="134" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A134" s="10"/>
       <c r="B134" s="10"/>
       <c r="C134" s="10"/>
@@ -25238,7 +25234,7 @@
       <c r="BS134" s="3"/>
       <c r="BT134" s="3"/>
     </row>
-    <row r="135" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A135" s="10"/>
       <c r="B135" s="10"/>
       <c r="C135" s="10"/>
@@ -25253,7 +25249,7 @@
       <c r="BS135" s="3"/>
       <c r="BT135" s="3"/>
     </row>
-    <row r="136" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN136" s="3"/>
       <c r="BO136" s="3"/>
       <c r="BP136" s="3"/>
@@ -25262,7 +25258,7 @@
       <c r="BS136" s="3"/>
       <c r="BT136" s="3"/>
     </row>
-    <row r="137" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN137" s="3"/>
       <c r="BO137" s="3"/>
       <c r="BP137" s="3"/>
@@ -25271,7 +25267,7 @@
       <c r="BS137" s="3"/>
       <c r="BT137" s="3"/>
     </row>
-    <row r="138" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN138" s="3"/>
       <c r="BO138" s="3"/>
       <c r="BP138" s="3"/>
@@ -25280,7 +25276,7 @@
       <c r="BS138" s="3"/>
       <c r="BT138" s="3"/>
     </row>
-    <row r="139" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN139" s="3"/>
       <c r="BO139" s="3"/>
       <c r="BP139" s="3"/>
@@ -25289,7 +25285,7 @@
       <c r="BS139" s="3"/>
       <c r="BT139" s="3"/>
     </row>
-    <row r="140" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN140" s="3"/>
       <c r="BO140" s="3"/>
       <c r="BP140" s="3"/>
@@ -25298,7 +25294,7 @@
       <c r="BS140" s="3"/>
       <c r="BT140" s="3"/>
     </row>
-    <row r="141" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN141" s="3"/>
       <c r="BO141" s="3"/>
       <c r="BP141" s="3"/>
@@ -25307,7 +25303,7 @@
       <c r="BS141" s="3"/>
       <c r="BT141" s="3"/>
     </row>
-    <row r="142" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A142" s="10"/>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -25322,7 +25318,7 @@
       <c r="BS142" s="3"/>
       <c r="BT142" s="3"/>
     </row>
-    <row r="143" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A143" s="10"/>
       <c r="B143" s="10"/>
       <c r="C143" s="10"/>
@@ -25337,7 +25333,7 @@
       <c r="BS143" s="3"/>
       <c r="BT143" s="3"/>
     </row>
-    <row r="144" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A144" s="10"/>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -25352,7 +25348,7 @@
       <c r="BS144" s="3"/>
       <c r="BT144" s="3"/>
     </row>
-    <row r="145" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A145" s="10"/>
       <c r="B145" s="10"/>
       <c r="C145" s="10"/>
@@ -25367,7 +25363,7 @@
       <c r="BS145" s="3"/>
       <c r="BT145" s="3"/>
     </row>
-    <row r="146" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A146" s="10"/>
       <c r="B146" s="10"/>
       <c r="C146" s="10"/>
@@ -25382,7 +25378,7 @@
       <c r="BS146" s="3"/>
       <c r="BT146" s="3"/>
     </row>
-    <row r="147" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A147" s="10"/>
       <c r="B147" s="10"/>
       <c r="C147" s="10"/>
@@ -25397,7 +25393,7 @@
       <c r="BS147" s="3"/>
       <c r="BT147" s="3"/>
     </row>
-    <row r="148" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:72" x14ac:dyDescent="0.25">
       <c r="AY148" s="1"/>
       <c r="BN148" s="3"/>
       <c r="BO148" s="3"/>
@@ -25407,7 +25403,7 @@
       <c r="BS148" s="3"/>
       <c r="BT148" s="3"/>
     </row>
-    <row r="149" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN149" s="3"/>
       <c r="BO149" s="3"/>
       <c r="BP149" s="3"/>
@@ -25416,7 +25412,7 @@
       <c r="BS149" s="3"/>
       <c r="BT149" s="3"/>
     </row>
-    <row r="150" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN150" s="3"/>
       <c r="BO150" s="3"/>
       <c r="BP150" s="3"/>
@@ -25425,7 +25421,7 @@
       <c r="BS150" s="3"/>
       <c r="BT150" s="3"/>
     </row>
-    <row r="151" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN151" s="3"/>
       <c r="BO151" s="3"/>
       <c r="BP151" s="3"/>
@@ -25434,7 +25430,7 @@
       <c r="BS151" s="3"/>
       <c r="BT151" s="3"/>
     </row>
-    <row r="152" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN152" s="3"/>
       <c r="BO152" s="3"/>
       <c r="BP152" s="3"/>
@@ -25443,7 +25439,7 @@
       <c r="BS152" s="3"/>
       <c r="BT152" s="3"/>
     </row>
-    <row r="153" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A153" s="10"/>
       <c r="B153" s="10"/>
       <c r="C153" s="10"/>
@@ -25458,7 +25454,7 @@
       <c r="BS153" s="3"/>
       <c r="BT153" s="3"/>
     </row>
-    <row r="154" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A154" s="10"/>
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
@@ -25473,7 +25469,7 @@
       <c r="BS154" s="3"/>
       <c r="BT154" s="3"/>
     </row>
-    <row r="155" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A155" s="10"/>
       <c r="B155" s="10"/>
       <c r="C155" s="10"/>
@@ -25488,7 +25484,7 @@
       <c r="BS155" s="3"/>
       <c r="BT155" s="3"/>
     </row>
-    <row r="156" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A156" s="10"/>
       <c r="B156" s="10"/>
       <c r="C156" s="10"/>
@@ -25503,7 +25499,7 @@
       <c r="BS156" s="3"/>
       <c r="BT156" s="3"/>
     </row>
-    <row r="157" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A157" s="10"/>
       <c r="B157" s="10"/>
       <c r="C157" s="10"/>
@@ -25518,7 +25514,7 @@
       <c r="BS157" s="3"/>
       <c r="BT157" s="3"/>
     </row>
-    <row r="158" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:72" x14ac:dyDescent="0.25">
       <c r="AY158" s="1"/>
       <c r="BN158" s="3"/>
       <c r="BO158" s="3"/>
@@ -25528,7 +25524,7 @@
       <c r="BS158" s="3"/>
       <c r="BT158" s="3"/>
     </row>
-    <row r="159" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN159" s="3"/>
       <c r="BO159" s="3"/>
       <c r="BP159" s="3"/>
@@ -25537,7 +25533,7 @@
       <c r="BS159" s="3"/>
       <c r="BT159" s="3"/>
     </row>
-    <row r="160" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN160" s="3"/>
       <c r="BO160" s="3"/>
       <c r="BP160" s="3"/>
@@ -25546,7 +25542,7 @@
       <c r="BS160" s="3"/>
       <c r="BT160" s="3"/>
     </row>
-    <row r="161" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN161" s="3"/>
       <c r="BO161" s="3"/>
       <c r="BP161" s="3"/>
@@ -25555,7 +25551,7 @@
       <c r="BS161" s="3"/>
       <c r="BT161" s="3"/>
     </row>
-    <row r="162" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN162" s="3"/>
       <c r="BO162" s="3"/>
       <c r="BP162" s="3"/>
@@ -25564,7 +25560,7 @@
       <c r="BS162" s="3"/>
       <c r="BT162" s="3"/>
     </row>
-    <row r="163" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A163" s="10"/>
       <c r="B163" s="10"/>
       <c r="C163" s="10"/>
@@ -25579,7 +25575,7 @@
       <c r="BS163" s="3"/>
       <c r="BT163" s="3"/>
     </row>
-    <row r="164" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A164" s="10"/>
       <c r="B164" s="10"/>
       <c r="C164" s="10"/>
@@ -25594,7 +25590,7 @@
       <c r="BS164" s="3"/>
       <c r="BT164" s="3"/>
     </row>
-    <row r="165" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A165" s="10"/>
       <c r="B165" s="10"/>
       <c r="C165" s="10"/>
@@ -25609,7 +25605,7 @@
       <c r="BS165" s="3"/>
       <c r="BT165" s="3"/>
     </row>
-    <row r="166" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A166" s="10"/>
       <c r="B166" s="10"/>
       <c r="C166" s="10"/>
@@ -25624,7 +25620,7 @@
       <c r="BS166" s="3"/>
       <c r="BT166" s="3"/>
     </row>
-    <row r="167" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A167" s="10"/>
       <c r="B167" s="10"/>
       <c r="C167" s="10"/>
@@ -25639,7 +25635,7 @@
       <c r="BS167" s="3"/>
       <c r="BT167" s="3"/>
     </row>
-    <row r="168" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A168" s="14"/>
       <c r="B168" s="14"/>
       <c r="C168" s="14"/>
@@ -25674,7 +25670,7 @@
       <c r="BS168" s="3"/>
       <c r="BT168" s="3"/>
     </row>
-    <row r="169" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN169" s="3"/>
       <c r="BO169" s="3"/>
       <c r="BP169" s="3"/>
@@ -25683,7 +25679,7 @@
       <c r="BS169" s="3"/>
       <c r="BT169" s="3"/>
     </row>
-    <row r="170" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN170" s="3"/>
       <c r="BO170" s="3"/>
       <c r="BP170" s="3"/>
@@ -25692,7 +25688,7 @@
       <c r="BS170" s="3"/>
       <c r="BT170" s="3"/>
     </row>
-    <row r="171" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BN171" s="3"/>
       <c r="BO171" s="3"/>
       <c r="BP171" s="3"/>
@@ -25701,7 +25697,7 @@
       <c r="BS171" s="3"/>
       <c r="BT171" s="3"/>
     </row>
-    <row r="172" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:72" x14ac:dyDescent="0.25">
       <c r="BC172" s="8"/>
       <c r="BN172" s="3"/>
       <c r="BO172" s="3"/>
@@ -25711,7 +25707,7 @@
       <c r="BS172" s="3"/>
       <c r="BT172" s="3"/>
     </row>
-    <row r="173" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A173" s="10"/>
       <c r="B173" s="10"/>
       <c r="C173" s="10"/>
@@ -25726,7 +25722,7 @@
       <c r="BS173" s="3"/>
       <c r="BT173" s="3"/>
     </row>
-    <row r="174" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A174" s="10"/>
       <c r="B174" s="10"/>
       <c r="C174" s="10"/>
@@ -25741,7 +25737,7 @@
       <c r="BS174" s="3"/>
       <c r="BT174" s="3"/>
     </row>
-    <row r="175" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A175" s="10"/>
       <c r="B175" s="10"/>
       <c r="C175" s="10"/>
@@ -25756,7 +25752,7 @@
       <c r="BS175" s="3"/>
       <c r="BT175" s="3"/>
     </row>
-    <row r="176" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A176" s="10"/>
       <c r="B176" s="10"/>
       <c r="C176" s="10"/>
@@ -25771,7 +25767,7 @@
       <c r="BS176" s="3"/>
       <c r="BT176" s="3"/>
     </row>
-    <row r="177" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A177" s="10"/>
       <c r="B177" s="10"/>
       <c r="C177" s="10"/>
@@ -25786,7 +25782,7 @@
       <c r="BS177" s="3"/>
       <c r="BT177" s="3"/>
     </row>
-    <row r="178" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A178" s="10"/>
       <c r="B178" s="10"/>
       <c r="C178" s="10"/>
@@ -25801,7 +25797,7 @@
       <c r="BS178" s="3"/>
       <c r="BT178" s="3"/>
     </row>
-    <row r="179" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -25876,7 +25872,7 @@
       <c r="BT179" s="2"/>
       <c r="BU179" s="1"/>
     </row>
-    <row r="180" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A180" s="7"/>
       <c r="BN180" s="3"/>
       <c r="BO180" s="3"/>
@@ -25886,7 +25882,7 @@
       <c r="BS180" s="3"/>
       <c r="BT180" s="3"/>
     </row>
-    <row r="181" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN181" s="3"/>
       <c r="BO181" s="3"/>
       <c r="BP181" s="3"/>
@@ -25895,7 +25891,7 @@
       <c r="BS181" s="3"/>
       <c r="BT181" s="3"/>
     </row>
-    <row r="182" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN182" s="3"/>
       <c r="BO182" s="3"/>
       <c r="BP182" s="3"/>
@@ -25904,7 +25900,7 @@
       <c r="BS182" s="3"/>
       <c r="BT182" s="3"/>
     </row>
-    <row r="183" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN183" s="3"/>
       <c r="BO183" s="3"/>
       <c r="BP183" s="3"/>
@@ -25913,7 +25909,7 @@
       <c r="BS183" s="3"/>
       <c r="BT183" s="3"/>
     </row>
-    <row r="184" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN184" s="3"/>
       <c r="BO184" s="3"/>
       <c r="BP184" s="3"/>
@@ -25922,7 +25918,7 @@
       <c r="BS184" s="3"/>
       <c r="BT184" s="3"/>
     </row>
-    <row r="185" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN185" s="3"/>
       <c r="BO185" s="3"/>
       <c r="BP185" s="3"/>
@@ -25931,7 +25927,7 @@
       <c r="BS185" s="3"/>
       <c r="BT185" s="3"/>
     </row>
-    <row r="186" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN186" s="3"/>
       <c r="BO186" s="3"/>
       <c r="BP186" s="3"/>
@@ -25940,7 +25936,7 @@
       <c r="BS186" s="3"/>
       <c r="BT186" s="3"/>
     </row>
-    <row r="187" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN187" s="3"/>
       <c r="BO187" s="3"/>
       <c r="BP187" s="3"/>
@@ -25949,7 +25945,7 @@
       <c r="BS187" s="3"/>
       <c r="BT187" s="3"/>
     </row>
-    <row r="188" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN188" s="3"/>
       <c r="BO188" s="3"/>
       <c r="BP188" s="3"/>
@@ -25958,7 +25954,7 @@
       <c r="BS188" s="3"/>
       <c r="BT188" s="3"/>
     </row>
-    <row r="189" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN189" s="3"/>
       <c r="BO189" s="3"/>
       <c r="BP189" s="3"/>
@@ -25967,7 +25963,7 @@
       <c r="BS189" s="3"/>
       <c r="BT189" s="3"/>
     </row>
-    <row r="190" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN190" s="3"/>
       <c r="BO190" s="3"/>
       <c r="BP190" s="3"/>
@@ -25976,7 +25972,7 @@
       <c r="BS190" s="3"/>
       <c r="BT190" s="3"/>
     </row>
-    <row r="191" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN191" s="3"/>
       <c r="BO191" s="3"/>
       <c r="BP191" s="3"/>
@@ -25985,7 +25981,7 @@
       <c r="BS191" s="3"/>
       <c r="BT191" s="3"/>
     </row>
-    <row r="192" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:73" x14ac:dyDescent="0.25">
       <c r="BN192" s="3"/>
       <c r="BO192" s="3"/>
       <c r="BP192" s="3"/>
@@ -25994,7 +25990,7 @@
       <c r="BS192" s="3"/>
       <c r="BT192" s="3"/>
     </row>
-    <row r="193" spans="66:72" x14ac:dyDescent="0.35">
+    <row r="193" spans="66:72" x14ac:dyDescent="0.25">
       <c r="BN193" s="3"/>
       <c r="BO193" s="3"/>
       <c r="BP193" s="3"/>
@@ -26003,7 +25999,7 @@
       <c r="BS193" s="3"/>
       <c r="BT193" s="3"/>
     </row>
-    <row r="194" spans="66:72" x14ac:dyDescent="0.35">
+    <row r="194" spans="66:72" x14ac:dyDescent="0.25">
       <c r="BN194" s="3"/>
       <c r="BO194" s="3"/>
       <c r="BP194" s="3"/>
@@ -26012,7 +26008,7 @@
       <c r="BS194" s="3"/>
       <c r="BT194" s="3"/>
     </row>
-    <row r="195" spans="66:72" x14ac:dyDescent="0.35">
+    <row r="195" spans="66:72" x14ac:dyDescent="0.25">
       <c r="BN195" s="3"/>
       <c r="BO195" s="3"/>
       <c r="BP195" s="3"/>

</xml_diff>